<commit_message>
Started working on the new event goal steps to allow for multiple event goals to play out back to back
</commit_message>
<xml_diff>
--- a/resources/data-imports/Npcs/npcs.xlsx
+++ b/resources/data-imports/Npcs/npcs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
   <si>
     <t>id</t>
   </si>
@@ -213,6 +213,18 @@
   </si>
   <si>
     <t>Grave Digger</t>
+  </si>
+  <si>
+    <t>TwistedCleric</t>
+  </si>
+  <si>
+    <t>Twisted Cleric</t>
+  </si>
+  <si>
+    <t>LonleyRedHawkSoldier</t>
+  </si>
+  <si>
+    <t>Lonley Red Hawk Soldier</t>
   </si>
 </sst>
 </file>
@@ -552,7 +564,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,8 +573,8 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="22.28" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="24.708" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="24.708" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="28.136" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="5.856" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="19.995" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="19.995" bestFit="true" customWidth="true" style="0"/>
@@ -1177,6 +1189,52 @@
       </c>
       <c r="J26">
         <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>61</v>
+      </c>
+      <c r="I27">
+        <v>384</v>
+      </c>
+      <c r="J27">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>61</v>
+      </c>
+      <c r="I28">
+        <v>368</v>
+      </c>
+      <c r="J28">
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new quests that lead up to the raid event for twisted memories plane
</commit_message>
<xml_diff>
--- a/resources/data-imports/Npcs/npcs.xlsx
+++ b/resources/data-imports/Npcs/npcs.xlsx
@@ -221,10 +221,10 @@
     <t>Twisted Cleric</t>
   </si>
   <si>
-    <t>LonleyRedHawkSoldier</t>
-  </si>
-  <si>
-    <t>Lonley Red Hawk Soldier</t>
+    <t>LonelyRedHawkSoldier</t>
+  </si>
+  <si>
+    <t>Lonely Red Hawk Soldier</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Comparison, item fixes and new NPC for conjuring celestials
</commit_message>
<xml_diff>
--- a/resources/data-imports/Npcs/npcs.xlsx
+++ b/resources/data-imports/Npcs/npcs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
   <si>
     <t>id</t>
   </si>
@@ -270,6 +270,12 @@
   </si>
   <si>
     <t>Haggard 'Ol Goblin</t>
+  </si>
+  <si>
+    <t>TheWitchofDelusions</t>
+  </si>
+  <si>
+    <t>The Witch of Delusions</t>
   </si>
 </sst>
 </file>
@@ -609,7 +615,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1443,6 +1449,29 @@
         <v>148</v>
       </c>
     </row>
+    <row r="36" spans="1:10">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>72</v>
+      </c>
+      <c r="I36">
+        <v>384</v>
+      </c>
+      <c r="J36">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added fixes to the way weekly fights happen, as well as a few other fixes here and there.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Npcs/npcs.xlsx
+++ b/resources/data-imports/Npcs/npcs.xlsx
@@ -131,7 +131,7 @@
     <t>Child of Shade</t>
   </si>
   <si>
-    <t>HellsGateKeeper</t>
+    <t>Hell'sGatekeeper</t>
   </si>
   <si>
     <t>Hell's Gatekeeper</t>
@@ -960,10 +960,10 @@
         <v>40</v>
       </c>
       <c r="I14">
-        <v>16</v>
+        <v>1552</v>
       </c>
       <c r="J14">
-        <v>336</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1420,10 +1420,10 @@
         <v>72</v>
       </c>
       <c r="I34">
-        <v>80</v>
+        <v>592</v>
       </c>
       <c r="J34">
-        <v>96</v>
+        <v>336</v>
       </c>
     </row>
     <row r="35" spans="1:10">

</xml_diff>

<commit_message>
Getting quests into place.
- Quests
- Quest Items
- New NPC's
- We can now choose a raid for when we generate events for development
- We can now set a proper position for NPC's on the admin map section.

Lots of other smaller fixes.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Npcs/npcs.xlsx
+++ b/resources/data-imports/Npcs/npcs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
   <si>
     <t>id</t>
   </si>
@@ -276,6 +276,18 @@
   </si>
   <si>
     <t>The Witch of Delusions</t>
+  </si>
+  <si>
+    <t>Mrs.Piper</t>
+  </si>
+  <si>
+    <t>Mrs. Piper</t>
+  </si>
+  <si>
+    <t>TheEnchantedSnowman</t>
+  </si>
+  <si>
+    <t>The Enchanted Snowman</t>
   </si>
 </sst>
 </file>
@@ -615,7 +627,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -684,10 +696,10 @@
         <v>12</v>
       </c>
       <c r="I2">
-        <v>96</v>
+        <v>384</v>
       </c>
       <c r="J2">
-        <v>192</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -707,10 +719,10 @@
         <v>12</v>
       </c>
       <c r="I3">
-        <v>160</v>
+        <v>288</v>
       </c>
       <c r="J3">
-        <v>80</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -730,10 +742,10 @@
         <v>12</v>
       </c>
       <c r="I4">
-        <v>464</v>
+        <v>1136</v>
       </c>
       <c r="J4">
-        <v>496</v>
+        <v>512</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -753,10 +765,10 @@
         <v>19</v>
       </c>
       <c r="I5">
-        <v>176</v>
+        <v>976</v>
       </c>
       <c r="J5">
-        <v>448</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -776,10 +788,10 @@
         <v>19</v>
       </c>
       <c r="I6">
-        <v>128</v>
+        <v>1040</v>
       </c>
       <c r="J6">
-        <v>384</v>
+        <v>592</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -799,10 +811,10 @@
         <v>19</v>
       </c>
       <c r="I7">
-        <v>112</v>
+        <v>1376</v>
       </c>
       <c r="J7">
-        <v>320</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -822,10 +834,10 @@
         <v>26</v>
       </c>
       <c r="I8">
-        <v>448</v>
+        <v>1344</v>
       </c>
       <c r="J8">
-        <v>96</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -845,10 +857,10 @@
         <v>12</v>
       </c>
       <c r="I9">
-        <v>32</v>
+        <v>1888</v>
       </c>
       <c r="J9">
-        <v>256</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -868,10 +880,10 @@
         <v>19</v>
       </c>
       <c r="I10">
-        <v>384</v>
+        <v>2016</v>
       </c>
       <c r="J10">
-        <v>496</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -891,10 +903,10 @@
         <v>33</v>
       </c>
       <c r="I11">
-        <v>288</v>
+        <v>784</v>
       </c>
       <c r="J11">
-        <v>480</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -914,10 +926,10 @@
         <v>26</v>
       </c>
       <c r="I12">
-        <v>384</v>
+        <v>688</v>
       </c>
       <c r="J12">
-        <v>368</v>
+        <v>512</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -960,10 +972,10 @@
         <v>40</v>
       </c>
       <c r="I14">
-        <v>1552</v>
+        <v>560</v>
       </c>
       <c r="J14">
-        <v>1392</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -983,10 +995,10 @@
         <v>40</v>
       </c>
       <c r="I15">
-        <v>432</v>
+        <v>864</v>
       </c>
       <c r="J15">
-        <v>80</v>
+        <v>608</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1006,10 +1018,10 @@
         <v>12</v>
       </c>
       <c r="I16">
-        <v>176</v>
+        <v>1072</v>
       </c>
       <c r="J16">
-        <v>144</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1029,10 +1041,10 @@
         <v>19</v>
       </c>
       <c r="I17">
-        <v>384</v>
+        <v>1696</v>
       </c>
       <c r="J17">
-        <v>64</v>
+        <v>496</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1052,10 +1064,10 @@
         <v>40</v>
       </c>
       <c r="I18">
-        <v>32</v>
+        <v>416</v>
       </c>
       <c r="J18">
-        <v>16</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1075,10 +1087,10 @@
         <v>40</v>
       </c>
       <c r="I19">
-        <v>16</v>
+        <v>1360</v>
       </c>
       <c r="J19">
-        <v>128</v>
+        <v>704</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1098,10 +1110,10 @@
         <v>26</v>
       </c>
       <c r="I20">
-        <v>96</v>
+        <v>304</v>
       </c>
       <c r="J20">
-        <v>496</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1121,10 +1133,10 @@
         <v>55</v>
       </c>
       <c r="I21">
-        <v>304</v>
+        <v>592</v>
       </c>
       <c r="J21">
-        <v>320</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1144,10 +1156,10 @@
         <v>55</v>
       </c>
       <c r="I22">
-        <v>64</v>
+        <v>1200</v>
       </c>
       <c r="J22">
-        <v>416</v>
+        <v>720</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1167,10 +1179,10 @@
         <v>55</v>
       </c>
       <c r="I23">
-        <v>16</v>
+        <v>1216</v>
       </c>
       <c r="J23">
-        <v>272</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1190,10 +1202,10 @@
         <v>61</v>
       </c>
       <c r="I24">
-        <v>32</v>
+        <v>944</v>
       </c>
       <c r="J24">
-        <v>304</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1213,10 +1225,10 @@
         <v>61</v>
       </c>
       <c r="I25">
-        <v>288</v>
+        <v>1328</v>
       </c>
       <c r="J25">
-        <v>304</v>
+        <v>496</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1236,10 +1248,10 @@
         <v>61</v>
       </c>
       <c r="I26">
-        <v>384</v>
+        <v>1008</v>
       </c>
       <c r="J26">
-        <v>32</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1259,10 +1271,10 @@
         <v>61</v>
       </c>
       <c r="I27">
-        <v>384</v>
+        <v>560</v>
       </c>
       <c r="J27">
-        <v>304</v>
+        <v>544</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1282,10 +1294,10 @@
         <v>61</v>
       </c>
       <c r="I28">
-        <v>368</v>
+        <v>1008</v>
       </c>
       <c r="J28">
-        <v>256</v>
+        <v>880</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1305,10 +1317,10 @@
         <v>72</v>
       </c>
       <c r="I29">
-        <v>112</v>
+        <v>1168</v>
       </c>
       <c r="J29">
-        <v>32</v>
+        <v>784</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1328,10 +1340,10 @@
         <v>72</v>
       </c>
       <c r="I30">
-        <v>448</v>
+        <v>736</v>
       </c>
       <c r="J30">
-        <v>320</v>
+        <v>944</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1351,10 +1363,10 @@
         <v>72</v>
       </c>
       <c r="I31">
-        <v>16</v>
+        <v>1280</v>
       </c>
       <c r="J31">
-        <v>224</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1374,10 +1386,10 @@
         <v>72</v>
       </c>
       <c r="I32">
-        <v>96</v>
+        <v>1760</v>
       </c>
       <c r="J32">
-        <v>432</v>
+        <v>400</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1397,10 +1409,10 @@
         <v>72</v>
       </c>
       <c r="I33">
-        <v>208</v>
+        <v>1344</v>
       </c>
       <c r="J33">
-        <v>416</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1443,10 +1455,10 @@
         <v>19</v>
       </c>
       <c r="I35">
-        <v>16</v>
+        <v>2336</v>
       </c>
       <c r="J35">
-        <v>148</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1466,10 +1478,56 @@
         <v>72</v>
       </c>
       <c r="I36">
-        <v>384</v>
+        <v>160</v>
       </c>
       <c r="J36">
-        <v>80</v>
+        <v>2192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>55</v>
+      </c>
+      <c r="I37">
+        <v>640</v>
+      </c>
+      <c r="J37">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>55</v>
+      </c>
+      <c r="I38">
+        <v>304</v>
+      </c>
+      <c r="J38">
+        <v>1232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new promotional material for the corrupted bishop. Various other changes
</commit_message>
<xml_diff>
--- a/resources/data-imports/Npcs/npcs.xlsx
+++ b/resources/data-imports/Npcs/npcs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
   <si>
     <t>id</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>The Frozen General</t>
+  </si>
+  <si>
+    <t>FrozenSoul</t>
+  </si>
+  <si>
+    <t>Frozen Soul</t>
   </si>
 </sst>
 </file>
@@ -633,7 +639,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1139,10 +1145,10 @@
         <v>55</v>
       </c>
       <c r="I21">
-        <v>592</v>
+        <v>192</v>
       </c>
       <c r="J21">
-        <v>1904</v>
+        <v>608</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1557,6 +1563,29 @@
       </c>
       <c r="J39">
         <v>736</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>55</v>
+      </c>
+      <c r="I40">
+        <v>336</v>
+      </c>
+      <c r="J40">
+        <v>1248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>